<commit_message>
fixed error in parsing
</commit_message>
<xml_diff>
--- a/히스토그램.xlsx
+++ b/히스토그램.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yonsei\biocomputing\assginment\Parsing Big Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B5B27F1-68D9-496D-B514-44043E15A9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F96C834-2F7D-41CB-93D3-249E85E6CB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{896E06CC-86B9-42B2-B40C-C9E9F65664E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{896E06CC-86B9-42B2-B40C-C9E9F65664E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MF</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>Path length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>path_MF [24, 190, 909, 2057, 5016, 1969, 765, 197, 38, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>path_BP [30, 438, 2318, 5159, 7079, 6658, 4270, 1811, 519, 160, 41, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>root제외 합계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -171,7 +183,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -200,6 +212,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -502,34 +520,34 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>437</c:v>
+                  <c:v>438</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2284</c:v>
+                  <c:v>2318</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5018</c:v>
+                  <c:v>5159</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7001</c:v>
+                  <c:v>7079</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6701</c:v>
+                  <c:v>6658</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4378</c:v>
+                  <c:v>4270</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1858</c:v>
+                  <c:v>1811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>561</c:v>
+                  <c:v>519</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>173</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1617,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45D79B3-9D2A-499A-847B-C5C0F3F8E819}">
-  <dimension ref="F6:I19"/>
+  <dimension ref="A6:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1661,7 +1679,7 @@
         <v>190</v>
       </c>
       <c r="I9" s="6">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="7:9" x14ac:dyDescent="0.3">
@@ -1672,7 +1690,7 @@
         <v>909</v>
       </c>
       <c r="I10" s="6">
-        <v>2284</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="11" spans="7:9" x14ac:dyDescent="0.3">
@@ -1683,7 +1701,7 @@
         <v>2057</v>
       </c>
       <c r="I11" s="6">
-        <v>5018</v>
+        <v>5159</v>
       </c>
     </row>
     <row r="12" spans="7:9" x14ac:dyDescent="0.3">
@@ -1694,7 +1712,7 @@
         <v>5016</v>
       </c>
       <c r="I12" s="6">
-        <v>7001</v>
+        <v>7079</v>
       </c>
     </row>
     <row r="13" spans="7:9" x14ac:dyDescent="0.3">
@@ -1705,7 +1723,7 @@
         <v>1969</v>
       </c>
       <c r="I13" s="6">
-        <v>6701</v>
+        <v>6658</v>
       </c>
     </row>
     <row r="14" spans="7:9" x14ac:dyDescent="0.3">
@@ -1716,7 +1734,7 @@
         <v>765</v>
       </c>
       <c r="I14" s="6">
-        <v>4378</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="15" spans="7:9" x14ac:dyDescent="0.3">
@@ -1727,7 +1745,7 @@
         <v>197</v>
       </c>
       <c r="I15" s="6">
-        <v>1858</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="16" spans="7:9" x14ac:dyDescent="0.3">
@@ -1738,10 +1756,10 @@
         <v>38</v>
       </c>
       <c r="I16" s="6">
-        <v>561</v>
+        <v>519</v>
       </c>
     </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G17" s="4">
         <v>10</v>
       </c>
@@ -1749,10 +1767,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="6">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="18" spans="7:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G18" s="7">
         <v>11</v>
       </c>
@@ -1760,11 +1778,53 @@
         <v>0</v>
       </c>
       <c r="I18" s="9">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="19" spans="7:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="10">
+        <f>SUM(H8:H18)</f>
+        <v>11165</v>
+      </c>
+      <c r="I19" s="10">
+        <f>SUM(I8:I18)</f>
+        <v>28483</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A23:I23"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1773,15 +1833,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101001A5760F8681D974EB944C00B284F4345" ma:contentTypeVersion="2" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="9c05d0383693eb0c653ee0cfca602f54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ed1e727f-bae2-4806-ba4f-a3d0adb19b4a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c512832dd1fcce304892706b3fa62a2a" ns3:_="">
     <xsd:import namespace="ed1e727f-bae2-4806-ba4f-a3d0adb19b4a"/>
@@ -1913,6 +1964,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1920,14 +1980,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{574A25AE-6D83-4F8E-BF17-DE5CF46903CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BBEA554-DFB1-44D5-9F31-6536D4A2ACE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1941,6 +1993,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{574A25AE-6D83-4F8E-BF17-DE5CF46903CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>